<commit_message>
Wed Aug 19 17:22:40 EDT 2020
</commit_message>
<xml_diff>
--- a/RadioVariableData.xlsx
+++ b/RadioVariableData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaguirre/Software/plimpy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258211E0-B8F0-AB47-A504-D627D41461CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17540B0-C9F9-F940-8D1B-E43E9015066D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9940" yWindow="460" windowWidth="21140" windowHeight="16840" xr2:uid="{267EDB05-8A74-3C49-B998-C79D35E21ED1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Reference</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Survey area</t>
   </si>
 </sst>
 </file>
@@ -423,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41119741-DB0C-FE42-A958-3962E0594898}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +456,11 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -473,7 +479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -490,7 +496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -508,7 +514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -526,7 +532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>7</v>
       </c>

</xml_diff>